<commit_message>
done with pci single sheet
</commit_message>
<xml_diff>
--- a/Audit_Code/public/PCI_DSS_4_Single_TSP.xlsx
+++ b/Audit_Code/public/PCI_DSS_4_Single_TSP.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\97154\OneDrive\Desktop\New2folder\AAAAAAA-Clients and Prospectives\GRC Abdullah\PCI sheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ab\Desktop\Compliance\Audit_Code\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{790929A5-917C-4C38-A097-778DCE49E3C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9630"/>
   </bookViews>
   <sheets>
     <sheet name="PCI DSS v4 sheet" sheetId="1" r:id="rId1"/>
@@ -18,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'PCI DSS v4 sheet'!$A$1:$F$257</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -2236,7 +2235,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2615,12 +2614,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BPW257"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A209" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A210" sqref="A210:XFD210"/>
+      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -6965,7 +6964,6 @@
         <v>3</v>
       </c>
       <c r="B43" s="4">
-        <f t="shared" ref="B43" si="0">B41+0.1</f>
         <v>3.4</v>
       </c>
       <c r="C43" s="3" t="s">
@@ -6984,7 +6982,6 @@
         <v>3</v>
       </c>
       <c r="B44" s="4">
-        <f t="shared" ref="B44" si="1">B42+0.1</f>
         <v>3.4</v>
       </c>
       <c r="C44" s="3" t="s">
@@ -8434,7 +8431,7 @@
       </c>
       <c r="F122" s="3"/>
     </row>
-    <row r="123" spans="1:6" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A123" s="4">
         <v>8</v>
       </c>
@@ -9330,7 +9327,7 @@
       </c>
       <c r="F171" s="3"/>
     </row>
-    <row r="172" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A172" s="4">
         <v>10</v>
       </c>
@@ -9366,7 +9363,7 @@
       </c>
       <c r="F173" s="3"/>
     </row>
-    <row r="174" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A174" s="4">
         <v>10</v>
       </c>
@@ -9384,7 +9381,7 @@
       </c>
       <c r="F174" s="3"/>
     </row>
-    <row r="175" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A175" s="4">
         <v>10</v>
       </c>
@@ -9438,7 +9435,7 @@
       </c>
       <c r="F177" s="3"/>
     </row>
-    <row r="178" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A178" s="4">
         <v>10</v>
       </c>
@@ -10166,7 +10163,7 @@
       </c>
       <c r="F217" s="3"/>
     </row>
-    <row r="218" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:6" ht="51" x14ac:dyDescent="0.25">
       <c r="A218" s="4">
         <v>12</v>
       </c>
@@ -10909,7 +10906,7 @@
       <c r="F257" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F257" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:F257"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>